<commit_message>
Added latest version of RTM
</commit_message>
<xml_diff>
--- a/Requirements Traceability Matrix (RTM).xlsx
+++ b/Requirements Traceability Matrix (RTM).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b45f31b031684218/Documents/CSC256GProject/RTM Requirement Matrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{9D0CB8EF-53A2-4D0A-9588-F65DCF429891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{505FC176-30EE-4630-AE88-71D14C25DBEE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C325479A-43FE-4773-9081-73FEB0213269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="5910" windowWidth="20205" windowHeight="14280" xr2:uid="{4B2A60C3-4E12-47F4-B400-566548060668}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,49 +36,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Requirement ID</t>
   </si>
   <si>
+    <t>Requirement Type</t>
+  </si>
+  <si>
     <t>Requirement Description</t>
   </si>
   <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
     <t>Test Case ID</t>
   </si>
   <si>
-    <t>Test Case Description</t>
-  </si>
-  <si>
     <t>Test Result</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Test if user can login</t>
+    <t>Remarks</t>
   </si>
   <si>
     <t xml:space="preserve">Ex: </t>
   </si>
   <si>
-    <t>TC-001</t>
-  </si>
-  <si>
-    <t>REQ-001</t>
-  </si>
-  <si>
-    <t>Comments</t>
+    <t>FR-001</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>User should be able to register for an account on the website</t>
+  </si>
+  <si>
+    <t>Register for an account and verify successful registration.</t>
+  </si>
+  <si>
+    <t>TC-FR-001</t>
+  </si>
+  <si>
+    <t>Pass or Fail</t>
+  </si>
+  <si>
+    <t>FR-002</t>
+  </si>
+  <si>
+    <t>Registered user must be able to login with credentials</t>
+  </si>
+  <si>
+    <t>Login with registered user credentials and verify successful login.</t>
+  </si>
+  <si>
+    <t>TC-FR-002</t>
+  </si>
+  <si>
+    <t>FR-003</t>
+  </si>
+  <si>
+    <t>User should be able to add products to their shopping cart, view, and proceed to check out.</t>
+  </si>
+  <si>
+    <t>Add products to the cart, verify cart contents, and proceed to the checkout page.</t>
+  </si>
+  <si>
+    <t>TC-FR-003</t>
+  </si>
+  <si>
+    <t>ER-001</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
+  <si>
+    <t>Test if an error message appears when trying to login with incorrect email ID or password.</t>
+  </si>
+  <si>
+    <t>Login with incorrect email or password and verify error message clearly appears.</t>
+  </si>
+  <si>
+    <t>TC-ER-001</t>
+  </si>
+  <si>
+    <t>REQ-004</t>
+  </si>
+  <si>
+    <t>REQ-006</t>
+  </si>
+  <si>
+    <t>REQ-007</t>
+  </si>
+  <si>
+    <t>REQ-008</t>
+  </si>
+  <si>
+    <t>REQ-009</t>
+  </si>
+  <si>
+    <t>REQ-010</t>
+  </si>
+  <si>
+    <t>REQ-011</t>
+  </si>
+  <si>
+    <t>REQ-012</t>
+  </si>
+  <si>
+    <t>REQ-013</t>
+  </si>
+  <si>
+    <t>REQ-014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,10 +212,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,23 +511,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDB30D3-E30C-4009-91D0-4A052D68A08D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="35.25" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -465,39 +538,361 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60.75">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45.75">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="76.5">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60.75">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F836F5720507947821BFD706B40BE67" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2232d5ccd5be264da3862beffe437d9c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b1f02aac-05c9-4520-9595-e03de4df9128" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef661f2d434a9b314c31d6fa1e355092" ns2:_="">
+    <xsd:import namespace="b1f02aac-05c9-4520-9595-e03de4df9128"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b1f02aac-05c9-4520-9595-e03de4df9128" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="52bd3d9c-d4ca-4556-be0e-df8152372c6f" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b1f02aac-05c9-4520-9595-e03de4df9128">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{133B2243-FC8C-4135-B25B-016086ADAC24}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F84A613-216F-4FFA-9C9E-E26E59428AD8}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F71BE8C-6E8A-41A1-9EC0-1FBC82BA7580}"/>
 </file>
</xml_diff>